<commit_message>
change reversal subject info
</commit_message>
<xml_diff>
--- a/rev_subject_order.xlsx
+++ b/rev_subject_order.xlsx
@@ -15,9 +15,9 @@
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="m f - Personal View" guid="{091B4786-2BDF-9F42-B31F-0DF6C7936D8F}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Eric Feltham - Personal View" guid="{7E9672F6-2B9F-3444-9E5C-118F130E07D4}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Jones, Natalie - Personal View" guid="{1EC22FF0-C7A3-4F9B-B884-8996B09914A6}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1456" windowHeight="876" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Eric Feltham - Personal View" guid="{7E9672F6-2B9F-3444-9E5C-118F130E07D4}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="m f - Personal View" guid="{091B4786-2BDF-9F42-B31F-0DF6C7936D8F}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3AD0B537-AE3B-5348-89FA-61580FDE6F1C}" diskRevisions="1" revisionId="416" version="50">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1FEBA539-A7C8-3D4E-8C41-A314239C175D}" diskRevisions="1" revisionId="418" version="51">
   <header guid="{A554BB17-C738-5B48-BAB0-21EC5378DDC6}" dateTime="2015-04-16T15:52:21" maxSheetId="2" userName="m f" r:id="rId7" minRId="23" maxRId="24">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -601,6 +601,11 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{1FEBA539-A7C8-3D4E-8C41-A314239C175D}" dateTime="2015-07-23T22:43:30" maxSheetId="2" userName="m f" r:id="rId53" minRId="417" maxRId="418">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3580,6 +3585,17 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog47.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="417" sId="1" eol="1" ref="A31:XFD31" action="insertRow"/>
+  <rcc rId="418" sId="1">
+    <nc r="A31">
+      <v>999</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="58" sId="1">
@@ -3739,7 +3755,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="9">
   <userInfo guid="{A554BB17-C738-5B48-BAB0-21EC5378DDC6}" name="Eric Feltham" id="-1854644501" dateTime="2015-04-20T10:23:06"/>
   <userInfo guid="{93004243-252E-EA4D-8D9B-3F72483E93D6}" name="Eric Feltham" id="-1854666493" dateTime="2015-07-08T11:10:22"/>
@@ -4075,10 +4091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5029,18 +5045,23 @@
         <v>18</v>
       </c>
     </row>
+    <row r="31" spans="1:16">
+      <c r="A31">
+        <v>999</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{1EC22FF0-C7A3-4F9B-B884-8996B09914A6}" showRuler="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <customSheetView guid="{091B4786-2BDF-9F42-B31F-0DF6C7936D8F}" topLeftCell="I1">
+      <selection activeCell="Q27" sqref="Q1:R1048576"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{7E9672F6-2B9F-3444-9E5C-118F130E07D4}">
       <selection activeCell="I19" sqref="I19"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{091B4786-2BDF-9F42-B31F-0DF6C7936D8F}" topLeftCell="I1">
-      <selection activeCell="Q27" sqref="Q1:R1048576"/>
+    <customSheetView guid="{1EC22FF0-C7A3-4F9B-B884-8996B09914A6}" showRuler="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>